<commit_message>
get file dir bug fix
</commit_message>
<xml_diff>
--- a/Results/FAIRnessResults-stageportal.xlsx
+++ b/Results/FAIRnessResults-stageportal.xlsx
@@ -1887,13 +1887,13 @@
     <col min="41" max="41" width="11.6328125" customWidth="true" bestFit="true"/>
     <col min="42" max="42" width="11.6328125" customWidth="true" bestFit="true"/>
     <col min="43" max="43" width="25.15625" customWidth="true" bestFit="true"/>
-    <col min="44" max="44" width="5.3359375" customWidth="true" bestFit="true"/>
+    <col min="44" max="44" width="7.3984375" customWidth="true" bestFit="true"/>
     <col min="45" max="45" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="46" max="46" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="47" max="47" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="48" max="48" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="49" max="49" width="10.28125" customWidth="true" bestFit="true"/>
-    <col min="50" max="50" width="5.3359375" customWidth="true" bestFit="true"/>
+    <col min="50" max="50" width="5.50390625" customWidth="true" bestFit="true"/>
     <col min="51" max="51" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="52" max="52" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="53" max="53" width="10.28125" customWidth="true" bestFit="true"/>
@@ -1902,7 +1902,7 @@
     <col min="56" max="56" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="57" max="57" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="58" max="58" width="10.28125" customWidth="true" bestFit="true"/>
-    <col min="59" max="59" width="5.3359375" customWidth="true" bestFit="true"/>
+    <col min="59" max="59" width="5.50390625" customWidth="true" bestFit="true"/>
     <col min="60" max="60" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="61" max="61" width="10.28125" customWidth="true" bestFit="true"/>
     <col min="62" max="62" width="10.28125" customWidth="true" bestFit="true"/>
@@ -2214,7 +2214,7 @@
       <c r="C2" t="n" s="4">
         <v>38.0</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2" t="n" s="4">
         <v>36.0</v>
       </c>
       <c r="E2" t="n" s="4">
@@ -2241,7 +2241,7 @@
       <c r="L2" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N2" t="n" s="4">
@@ -2256,7 +2256,7 @@
       <c r="Q2" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R2" t="n">
+      <c r="R2" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S2" t="n" s="4">
@@ -2268,7 +2268,7 @@
       <c r="U2" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V2" t="n">
+      <c r="V2" t="n" s="4">
         <v>20.0</v>
       </c>
       <c r="W2" t="n" s="4">
@@ -2283,7 +2283,7 @@
       <c r="Z2" t="n" s="4">
         <v>76.0</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AA2" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB2" t="n" s="4">
@@ -2298,7 +2298,7 @@
       <c r="AE2" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AF2" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG2" t="n" s="4">
@@ -2307,7 +2307,7 @@
       <c r="AH2" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AI2" t="n" s="4">
         <v>45.0</v>
       </c>
       <c r="AJ2" t="n" s="4">
@@ -2316,7 +2316,7 @@
       <c r="AK2" t="n" s="4">
         <v>6.0</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="AL2" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM2" t="n" s="4">
@@ -2334,7 +2334,7 @@
       <c r="AQ2" t="n" s="4">
         <v>58.0</v>
       </c>
-      <c r="AR2" t="n">
+      <c r="AR2" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS2" t="n" s="4">
@@ -2352,7 +2352,7 @@
       <c r="AW2" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX2" t="n">
+      <c r="AX2" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY2" t="n" s="4">
@@ -2379,7 +2379,7 @@
       <c r="BF2" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG2" t="n">
+      <c r="BG2" t="n" s="4">
         <v>33.0</v>
       </c>
       <c r="BH2" t="n" s="4">
@@ -2400,7 +2400,7 @@
       <c r="BM2" t="n" s="4">
         <v>44.0</v>
       </c>
-      <c r="BN2" t="n">
+      <c r="BN2" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO2" t="n" s="4">
@@ -2415,7 +2415,7 @@
       <c r="BR2" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS2" t="n">
+      <c r="BS2" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="BT2" t="n" s="4">
@@ -2430,7 +2430,7 @@
       <c r="BW2" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX2" t="n">
+      <c r="BX2" t="n" s="4">
         <v>34.0</v>
       </c>
       <c r="BY2" t="n" s="4">
@@ -2451,7 +2451,7 @@
       <c r="CD2" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="CE2" t="n">
+      <c r="CE2" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF2" t="n" s="4">
@@ -2483,7 +2483,7 @@
       <c r="C3" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E3" t="n" s="4">
@@ -2510,7 +2510,7 @@
       <c r="L3" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N3" t="n" s="4">
@@ -2525,7 +2525,7 @@
       <c r="Q3" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R3" t="n">
+      <c r="R3" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S3" t="n" s="4">
@@ -2537,7 +2537,7 @@
       <c r="U3" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V3" t="n">
+      <c r="V3" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W3" t="n" s="4">
@@ -2552,7 +2552,7 @@
       <c r="Z3" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AA3" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB3" t="n" s="4">
@@ -2567,7 +2567,7 @@
       <c r="AE3" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AF3" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG3" t="n" s="4">
@@ -2576,7 +2576,7 @@
       <c r="AH3" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AI3" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ3" t="n" s="4">
@@ -2585,7 +2585,7 @@
       <c r="AK3" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL3" t="n">
+      <c r="AL3" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM3" t="n" s="4">
@@ -2603,7 +2603,7 @@
       <c r="AQ3" t="n" s="4">
         <v>49.0</v>
       </c>
-      <c r="AR3" t="n">
+      <c r="AR3" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AS3" t="n" s="4">
@@ -2621,7 +2621,7 @@
       <c r="AW3" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX3" t="n">
+      <c r="AX3" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY3" t="n" s="4">
@@ -2648,7 +2648,7 @@
       <c r="BF3" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG3" t="n">
+      <c r="BG3" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH3" t="n" s="4">
@@ -2669,7 +2669,7 @@
       <c r="BM3" t="n" s="4">
         <v>23.0</v>
       </c>
-      <c r="BN3" t="n">
+      <c r="BN3" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO3" t="n" s="4">
@@ -2684,7 +2684,7 @@
       <c r="BR3" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS3" t="n">
+      <c r="BS3" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT3" t="n" s="4">
@@ -2699,7 +2699,7 @@
       <c r="BW3" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX3" t="n">
+      <c r="BX3" t="n" s="4">
         <v>4.0</v>
       </c>
       <c r="BY3" t="n" s="4">
@@ -2720,7 +2720,7 @@
       <c r="CD3" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE3" t="n">
+      <c r="CE3" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF3" t="n" s="4">
@@ -2752,7 +2752,7 @@
       <c r="C4" t="n" s="4">
         <v>42.0</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4" t="n" s="4">
         <v>51.0</v>
       </c>
       <c r="E4" t="n" s="4">
@@ -2779,7 +2779,7 @@
       <c r="L4" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M4" t="n">
+      <c r="M4" t="n" s="4">
         <v>88.0</v>
       </c>
       <c r="N4" t="n" s="4">
@@ -2794,7 +2794,7 @@
       <c r="Q4" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R4" t="n">
+      <c r="R4" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S4" t="n" s="4">
@@ -2806,7 +2806,7 @@
       <c r="U4" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V4" t="n">
+      <c r="V4" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W4" t="n" s="4">
@@ -2821,7 +2821,7 @@
       <c r="Z4" t="n" s="4">
         <v>76.0</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AA4" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AB4" t="n" s="4">
@@ -2836,7 +2836,7 @@
       <c r="AE4" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AF4" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG4" t="n" s="4">
@@ -2845,7 +2845,7 @@
       <c r="AH4" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AI4" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ4" t="n" s="4">
@@ -2854,7 +2854,7 @@
       <c r="AK4" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL4" t="n">
+      <c r="AL4" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM4" t="n" s="4">
@@ -2872,7 +2872,7 @@
       <c r="AQ4" t="n" s="4">
         <v>55.0</v>
       </c>
-      <c r="AR4" t="n">
+      <c r="AR4" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS4" t="n" s="4">
@@ -2890,7 +2890,7 @@
       <c r="AW4" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX4" t="n">
+      <c r="AX4" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY4" t="n" s="4">
@@ -2917,7 +2917,7 @@
       <c r="BF4" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG4" t="n">
+      <c r="BG4" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH4" t="n" s="4">
@@ -2938,7 +2938,7 @@
       <c r="BM4" t="n" s="4">
         <v>38.0</v>
       </c>
-      <c r="BN4" t="n">
+      <c r="BN4" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO4" t="n" s="4">
@@ -2953,7 +2953,7 @@
       <c r="BR4" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS4" t="n">
+      <c r="BS4" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="BT4" t="n" s="4">
@@ -2968,7 +2968,7 @@
       <c r="BW4" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX4" t="n">
+      <c r="BX4" t="n" s="4">
         <v>8.0</v>
       </c>
       <c r="BY4" t="n" s="4">
@@ -2989,7 +2989,7 @@
       <c r="CD4" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE4" t="n">
+      <c r="CE4" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF4" t="n" s="4">
@@ -3021,7 +3021,7 @@
       <c r="C5" t="n" s="4">
         <v>36.0</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5" t="n" s="4">
         <v>36.0</v>
       </c>
       <c r="E5" t="n" s="4">
@@ -3048,7 +3048,7 @@
       <c r="L5" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M5" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N5" t="n" s="4">
@@ -3063,7 +3063,7 @@
       <c r="Q5" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R5" t="n">
+      <c r="R5" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S5" t="n" s="4">
@@ -3075,7 +3075,7 @@
       <c r="U5" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V5" t="n">
+      <c r="V5" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W5" t="n" s="4">
@@ -3090,7 +3090,7 @@
       <c r="Z5" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AA5" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB5" t="n" s="4">
@@ -3105,7 +3105,7 @@
       <c r="AE5" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AF5" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG5" t="n" s="4">
@@ -3114,7 +3114,7 @@
       <c r="AH5" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AI5" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ5" t="n" s="4">
@@ -3123,7 +3123,7 @@
       <c r="AK5" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="AL5" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM5" t="n" s="4">
@@ -3141,7 +3141,7 @@
       <c r="AQ5" t="n" s="4">
         <v>58.0</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="AR5" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS5" t="n" s="4">
@@ -3159,7 +3159,7 @@
       <c r="AW5" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX5" t="n">
+      <c r="AX5" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY5" t="n" s="4">
@@ -3186,7 +3186,7 @@
       <c r="BF5" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG5" t="n">
+      <c r="BG5" t="n" s="4">
         <v>33.0</v>
       </c>
       <c r="BH5" t="n" s="4">
@@ -3207,7 +3207,7 @@
       <c r="BM5" t="n" s="4">
         <v>39.0</v>
       </c>
-      <c r="BN5" t="n">
+      <c r="BN5" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO5" t="n" s="4">
@@ -3222,7 +3222,7 @@
       <c r="BR5" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS5" t="n">
+      <c r="BS5" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="BT5" t="n" s="4">
@@ -3237,7 +3237,7 @@
       <c r="BW5" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX5" t="n">
+      <c r="BX5" t="n" s="4">
         <v>13.0</v>
       </c>
       <c r="BY5" t="n" s="4">
@@ -3258,7 +3258,7 @@
       <c r="CD5" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE5" t="n">
+      <c r="CE5" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF5" t="n" s="4">
@@ -3290,7 +3290,7 @@
       <c r="C6" t="n" s="4">
         <v>41.0</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6" t="n" s="4">
         <v>51.0</v>
       </c>
       <c r="E6" t="n" s="4">
@@ -3317,7 +3317,7 @@
       <c r="L6" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M6" t="n">
+      <c r="M6" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N6" t="n" s="4">
@@ -3332,7 +3332,7 @@
       <c r="Q6" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R6" t="n">
+      <c r="R6" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S6" t="n" s="4">
@@ -3344,7 +3344,7 @@
       <c r="U6" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V6" t="n">
+      <c r="V6" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W6" t="n" s="4">
@@ -3359,7 +3359,7 @@
       <c r="Z6" t="n" s="4">
         <v>76.0</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AA6" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AB6" t="n" s="4">
@@ -3374,7 +3374,7 @@
       <c r="AE6" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AF6" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG6" t="n" s="4">
@@ -3383,7 +3383,7 @@
       <c r="AH6" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AI6" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ6" t="n" s="4">
@@ -3392,7 +3392,7 @@
       <c r="AK6" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL6" t="n">
+      <c r="AL6" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM6" t="n" s="4">
@@ -3410,7 +3410,7 @@
       <c r="AQ6" t="n" s="4">
         <v>55.0</v>
       </c>
-      <c r="AR6" t="n">
+      <c r="AR6" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS6" t="n" s="4">
@@ -3428,7 +3428,7 @@
       <c r="AW6" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX6" t="n">
+      <c r="AX6" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY6" t="n" s="4">
@@ -3455,7 +3455,7 @@
       <c r="BF6" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG6" t="n">
+      <c r="BG6" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH6" t="n" s="4">
@@ -3476,7 +3476,7 @@
       <c r="BM6" t="n" s="4">
         <v>29.0</v>
       </c>
-      <c r="BN6" t="n">
+      <c r="BN6" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO6" t="n" s="4">
@@ -3491,7 +3491,7 @@
       <c r="BR6" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS6" t="n">
+      <c r="BS6" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT6" t="n" s="4">
@@ -3506,7 +3506,7 @@
       <c r="BW6" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX6" t="n">
+      <c r="BX6" t="n" s="4">
         <v>17.0</v>
       </c>
       <c r="BY6" t="n" s="4">
@@ -3527,7 +3527,7 @@
       <c r="CD6" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE6" t="n">
+      <c r="CE6" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF6" t="n" s="4">
@@ -3559,7 +3559,7 @@
       <c r="C7" t="n" s="4">
         <v>47.0</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7" t="n" s="4">
         <v>63.0</v>
       </c>
       <c r="E7" t="n" s="4">
@@ -3586,7 +3586,7 @@
       <c r="L7" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M7" t="n">
+      <c r="M7" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N7" t="n" s="4">
@@ -3601,7 +3601,7 @@
       <c r="Q7" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R7" t="n">
+      <c r="R7" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S7" t="n" s="4">
@@ -3613,7 +3613,7 @@
       <c r="U7" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V7" t="n">
+      <c r="V7" t="n" s="4">
         <v>20.0</v>
       </c>
       <c r="W7" t="n" s="4">
@@ -3628,7 +3628,7 @@
       <c r="Z7" t="n" s="4">
         <v>81.0</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AA7" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AB7" t="n" s="4">
@@ -3643,7 +3643,7 @@
       <c r="AE7" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AF7" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG7" t="n" s="4">
@@ -3652,7 +3652,7 @@
       <c r="AH7" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AI7" t="n" s="4">
         <v>45.0</v>
       </c>
       <c r="AJ7" t="n" s="4">
@@ -3661,7 +3661,7 @@
       <c r="AK7" t="n" s="4">
         <v>6.0</v>
       </c>
-      <c r="AL7" t="n">
+      <c r="AL7" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM7" t="n" s="4">
@@ -3679,7 +3679,7 @@
       <c r="AQ7" t="n" s="4">
         <v>56.0</v>
       </c>
-      <c r="AR7" t="n">
+      <c r="AR7" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AS7" t="n" s="4">
@@ -3697,7 +3697,7 @@
       <c r="AW7" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX7" t="n">
+      <c r="AX7" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY7" t="n" s="4">
@@ -3724,7 +3724,7 @@
       <c r="BF7" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG7" t="n">
+      <c r="BG7" t="n" s="4">
         <v>33.0</v>
       </c>
       <c r="BH7" t="n" s="4">
@@ -3745,7 +3745,7 @@
       <c r="BM7" t="n" s="4">
         <v>38.0</v>
       </c>
-      <c r="BN7" t="n">
+      <c r="BN7" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO7" t="n" s="4">
@@ -3760,7 +3760,7 @@
       <c r="BR7" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS7" t="n">
+      <c r="BS7" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="BT7" t="n" s="4">
@@ -3775,7 +3775,7 @@
       <c r="BW7" t="n" s="4">
         <v>10.0</v>
       </c>
-      <c r="BX7" t="n">
+      <c r="BX7" t="n" s="4">
         <v>8.0</v>
       </c>
       <c r="BY7" t="n" s="4">
@@ -3796,7 +3796,7 @@
       <c r="CD7" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE7" t="n">
+      <c r="CE7" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF7" t="n" s="4">
@@ -3828,7 +3828,7 @@
       <c r="C8" t="n" s="4">
         <v>38.0</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8" t="n" s="4">
         <v>36.0</v>
       </c>
       <c r="E8" t="n" s="4">
@@ -3855,7 +3855,7 @@
       <c r="L8" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M8" t="n">
+      <c r="M8" t="n" s="4">
         <v>88.0</v>
       </c>
       <c r="N8" t="n" s="4">
@@ -3870,7 +3870,7 @@
       <c r="Q8" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R8" t="n">
+      <c r="R8" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S8" t="n" s="4">
@@ -3882,7 +3882,7 @@
       <c r="U8" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V8" t="n">
+      <c r="V8" t="n" s="4">
         <v>20.0</v>
       </c>
       <c r="W8" t="n" s="4">
@@ -3897,7 +3897,7 @@
       <c r="Z8" t="n" s="4">
         <v>76.0</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AA8" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB8" t="n" s="4">
@@ -3912,7 +3912,7 @@
       <c r="AE8" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF8" t="n">
+      <c r="AF8" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG8" t="n" s="4">
@@ -3921,7 +3921,7 @@
       <c r="AH8" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI8" t="n">
+      <c r="AI8" t="n" s="4">
         <v>45.0</v>
       </c>
       <c r="AJ8" t="n" s="4">
@@ -3930,7 +3930,7 @@
       <c r="AK8" t="n" s="4">
         <v>6.0</v>
       </c>
-      <c r="AL8" t="n">
+      <c r="AL8" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM8" t="n" s="4">
@@ -3948,7 +3948,7 @@
       <c r="AQ8" t="n" s="4">
         <v>54.0</v>
       </c>
-      <c r="AR8" t="n">
+      <c r="AR8" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS8" t="n" s="4">
@@ -3966,7 +3966,7 @@
       <c r="AW8" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX8" t="n">
+      <c r="AX8" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY8" t="n" s="4">
@@ -3993,7 +3993,7 @@
       <c r="BF8" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG8" t="n">
+      <c r="BG8" t="n" s="4">
         <v>33.0</v>
       </c>
       <c r="BH8" t="n" s="4">
@@ -4014,7 +4014,7 @@
       <c r="BM8" t="n" s="4">
         <v>43.0</v>
       </c>
-      <c r="BN8" t="n">
+      <c r="BN8" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO8" t="n" s="4">
@@ -4029,7 +4029,7 @@
       <c r="BR8" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS8" t="n">
+      <c r="BS8" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="BT8" t="n" s="4">
@@ -4044,7 +4044,7 @@
       <c r="BW8" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX8" t="n">
+      <c r="BX8" t="n" s="4">
         <v>29.0</v>
       </c>
       <c r="BY8" t="n" s="4">
@@ -4065,7 +4065,7 @@
       <c r="CD8" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="CE8" t="n">
+      <c r="CE8" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF8" t="n" s="4">
@@ -4097,7 +4097,7 @@
       <c r="C9" t="n" s="4">
         <v>31.0</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9" t="n" s="4">
         <v>21.0</v>
       </c>
       <c r="E9" t="n" s="4">
@@ -4124,7 +4124,7 @@
       <c r="L9" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M9" t="n">
+      <c r="M9" t="n" s="4">
         <v>88.0</v>
       </c>
       <c r="N9" t="n" s="4">
@@ -4139,7 +4139,7 @@
       <c r="Q9" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R9" t="n">
+      <c r="R9" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S9" t="n" s="4">
@@ -4151,7 +4151,7 @@
       <c r="U9" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V9" t="n">
+      <c r="V9" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W9" t="n" s="4">
@@ -4166,7 +4166,7 @@
       <c r="Z9" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AA9" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB9" t="n" s="4">
@@ -4181,7 +4181,7 @@
       <c r="AE9" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AF9" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG9" t="n" s="4">
@@ -4190,7 +4190,7 @@
       <c r="AH9" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AI9" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ9" t="n" s="4">
@@ -4199,7 +4199,7 @@
       <c r="AK9" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL9" t="n">
+      <c r="AL9" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM9" t="n" s="4">
@@ -4217,7 +4217,7 @@
       <c r="AQ9" t="n" s="4">
         <v>59.0</v>
       </c>
-      <c r="AR9" t="n">
+      <c r="AR9" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AS9" t="n" s="4">
@@ -4235,7 +4235,7 @@
       <c r="AW9" t="n" s="4">
         <v>4.0</v>
       </c>
-      <c r="AX9" t="n">
+      <c r="AX9" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY9" t="n" s="4">
@@ -4262,7 +4262,7 @@
       <c r="BF9" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG9" t="n">
+      <c r="BG9" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH9" t="n" s="4">
@@ -4283,7 +4283,7 @@
       <c r="BM9" t="n" s="4">
         <v>58.0</v>
       </c>
-      <c r="BN9" t="n">
+      <c r="BN9" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO9" t="n" s="4">
@@ -4298,7 +4298,7 @@
       <c r="BR9" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS9" t="n">
+      <c r="BS9" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="BT9" t="n" s="4">
@@ -4313,7 +4313,7 @@
       <c r="BW9" t="n" s="4">
         <v>15.0</v>
       </c>
-      <c r="BX9" t="n">
+      <c r="BX9" t="n" s="4">
         <v>60.0</v>
       </c>
       <c r="BY9" t="n" s="4">
@@ -4334,7 +4334,7 @@
       <c r="CD9" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="CE9" t="n">
+      <c r="CE9" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF9" t="n" s="4">
@@ -4366,7 +4366,7 @@
       <c r="C10" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E10" t="n" s="4">
@@ -4393,7 +4393,7 @@
       <c r="L10" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M10" t="n">
+      <c r="M10" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N10" t="n" s="4">
@@ -4408,7 +4408,7 @@
       <c r="Q10" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R10" t="n">
+      <c r="R10" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S10" t="n" s="4">
@@ -4420,7 +4420,7 @@
       <c r="U10" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V10" t="n">
+      <c r="V10" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W10" t="n" s="4">
@@ -4435,7 +4435,7 @@
       <c r="Z10" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AA10" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB10" t="n" s="4">
@@ -4450,7 +4450,7 @@
       <c r="AE10" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF10" t="n">
+      <c r="AF10" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG10" t="n" s="4">
@@ -4459,7 +4459,7 @@
       <c r="AH10" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI10" t="n">
+      <c r="AI10" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ10" t="n" s="4">
@@ -4468,7 +4468,7 @@
       <c r="AK10" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL10" t="n">
+      <c r="AL10" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM10" t="n" s="4">
@@ -4486,7 +4486,7 @@
       <c r="AQ10" t="n" s="4">
         <v>55.0</v>
       </c>
-      <c r="AR10" t="n">
+      <c r="AR10" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AS10" t="n" s="4">
@@ -4504,7 +4504,7 @@
       <c r="AW10" t="n" s="4">
         <v>4.0</v>
       </c>
-      <c r="AX10" t="n">
+      <c r="AX10" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY10" t="n" s="4">
@@ -4531,7 +4531,7 @@
       <c r="BF10" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG10" t="n">
+      <c r="BG10" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH10" t="n" s="4">
@@ -4552,7 +4552,7 @@
       <c r="BM10" t="n" s="4">
         <v>43.0</v>
       </c>
-      <c r="BN10" t="n">
+      <c r="BN10" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO10" t="n" s="4">
@@ -4567,7 +4567,7 @@
       <c r="BR10" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS10" t="n">
+      <c r="BS10" t="n" s="4">
         <v>54.0</v>
       </c>
       <c r="BT10" t="n" s="4">
@@ -4582,7 +4582,7 @@
       <c r="BW10" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX10" t="n">
+      <c r="BX10" t="n" s="4">
         <v>46.0</v>
       </c>
       <c r="BY10" t="n" s="4">
@@ -4603,7 +4603,7 @@
       <c r="CD10" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE10" t="n">
+      <c r="CE10" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF10" t="n" s="4">
@@ -4635,7 +4635,7 @@
       <c r="C11" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E11" t="n" s="4">
@@ -4662,7 +4662,7 @@
       <c r="L11" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M11" t="n">
+      <c r="M11" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N11" t="n" s="4">
@@ -4677,7 +4677,7 @@
       <c r="Q11" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R11" t="n">
+      <c r="R11" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S11" t="n" s="4">
@@ -4689,7 +4689,7 @@
       <c r="U11" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V11" t="n">
+      <c r="V11" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W11" t="n" s="4">
@@ -4704,7 +4704,7 @@
       <c r="Z11" t="n" s="4">
         <v>64.0</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AA11" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB11" t="n" s="4">
@@ -4719,7 +4719,7 @@
       <c r="AE11" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF11" t="n">
+      <c r="AF11" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG11" t="n" s="4">
@@ -4728,7 +4728,7 @@
       <c r="AH11" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI11" t="n">
+      <c r="AI11" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ11" t="n" s="4">
@@ -4737,7 +4737,7 @@
       <c r="AK11" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL11" t="n">
+      <c r="AL11" t="n" s="4">
         <v>50.0</v>
       </c>
       <c r="AM11" t="n" s="4">
@@ -4755,7 +4755,7 @@
       <c r="AQ11" t="n" s="4">
         <v>51.0</v>
       </c>
-      <c r="AR11" t="n">
+      <c r="AR11" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS11" t="n" s="4">
@@ -4773,7 +4773,7 @@
       <c r="AW11" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX11" t="n">
+      <c r="AX11" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY11" t="n" s="4">
@@ -4800,7 +4800,7 @@
       <c r="BF11" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG11" t="n">
+      <c r="BG11" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH11" t="n" s="4">
@@ -4821,7 +4821,7 @@
       <c r="BM11" t="n" s="4">
         <v>23.0</v>
       </c>
-      <c r="BN11" t="n">
+      <c r="BN11" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO11" t="n" s="4">
@@ -4836,7 +4836,7 @@
       <c r="BR11" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS11" t="n">
+      <c r="BS11" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT11" t="n" s="4">
@@ -4851,7 +4851,7 @@
       <c r="BW11" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX11" t="n">
+      <c r="BX11" t="n" s="4">
         <v>4.0</v>
       </c>
       <c r="BY11" t="n" s="4">
@@ -4872,7 +4872,7 @@
       <c r="CD11" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE11" t="n">
+      <c r="CE11" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF11" t="n" s="4">
@@ -4904,7 +4904,7 @@
       <c r="C12" t="n" s="4">
         <v>41.0</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12" t="n" s="4">
         <v>51.0</v>
       </c>
       <c r="E12" t="n" s="4">
@@ -4931,7 +4931,7 @@
       <c r="L12" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M12" t="n">
+      <c r="M12" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N12" t="n" s="4">
@@ -4946,7 +4946,7 @@
       <c r="Q12" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R12" t="n">
+      <c r="R12" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S12" t="n" s="4">
@@ -4958,7 +4958,7 @@
       <c r="U12" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V12" t="n">
+      <c r="V12" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W12" t="n" s="4">
@@ -4973,7 +4973,7 @@
       <c r="Z12" t="n" s="4">
         <v>76.0</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AA12" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AB12" t="n" s="4">
@@ -4988,7 +4988,7 @@
       <c r="AE12" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF12" t="n">
+      <c r="AF12" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG12" t="n" s="4">
@@ -4997,7 +4997,7 @@
       <c r="AH12" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI12" t="n">
+      <c r="AI12" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ12" t="n" s="4">
@@ -5006,7 +5006,7 @@
       <c r="AK12" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL12" t="n">
+      <c r="AL12" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM12" t="n" s="4">
@@ -5024,7 +5024,7 @@
       <c r="AQ12" t="n" s="4">
         <v>51.0</v>
       </c>
-      <c r="AR12" t="n">
+      <c r="AR12" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS12" t="n" s="4">
@@ -5042,7 +5042,7 @@
       <c r="AW12" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX12" t="n">
+      <c r="AX12" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY12" t="n" s="4">
@@ -5069,7 +5069,7 @@
       <c r="BF12" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG12" t="n">
+      <c r="BG12" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH12" t="n" s="4">
@@ -5090,7 +5090,7 @@
       <c r="BM12" t="n" s="4">
         <v>27.0</v>
       </c>
-      <c r="BN12" t="n">
+      <c r="BN12" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO12" t="n" s="4">
@@ -5105,7 +5105,7 @@
       <c r="BR12" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS12" t="n">
+      <c r="BS12" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT12" t="n" s="4">
@@ -5120,7 +5120,7 @@
       <c r="BW12" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX12" t="n">
+      <c r="BX12" t="n" s="4">
         <v>8.0</v>
       </c>
       <c r="BY12" t="n" s="4">
@@ -5141,7 +5141,7 @@
       <c r="CD12" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE12" t="n">
+      <c r="CE12" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF12" t="n" s="4">
@@ -5173,7 +5173,7 @@
       <c r="C13" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E13" t="n" s="4">
@@ -5200,7 +5200,7 @@
       <c r="L13" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M13" t="n">
+      <c r="M13" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N13" t="n" s="4">
@@ -5215,7 +5215,7 @@
       <c r="Q13" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R13" t="n">
+      <c r="R13" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S13" t="n" s="4">
@@ -5227,7 +5227,7 @@
       <c r="U13" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V13" t="n">
+      <c r="V13" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W13" t="n" s="4">
@@ -5242,7 +5242,7 @@
       <c r="Z13" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AA13" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB13" t="n" s="4">
@@ -5257,7 +5257,7 @@
       <c r="AE13" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF13" t="n">
+      <c r="AF13" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG13" t="n" s="4">
@@ -5266,7 +5266,7 @@
       <c r="AH13" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI13" t="n">
+      <c r="AI13" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ13" t="n" s="4">
@@ -5275,7 +5275,7 @@
       <c r="AK13" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL13" t="n">
+      <c r="AL13" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM13" t="n" s="4">
@@ -5293,7 +5293,7 @@
       <c r="AQ13" t="n" s="4">
         <v>56.0</v>
       </c>
-      <c r="AR13" t="n">
+      <c r="AR13" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AS13" t="n" s="4">
@@ -5311,7 +5311,7 @@
       <c r="AW13" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX13" t="n">
+      <c r="AX13" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY13" t="n" s="4">
@@ -5338,7 +5338,7 @@
       <c r="BF13" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG13" t="n">
+      <c r="BG13" t="n" s="4">
         <v>33.0</v>
       </c>
       <c r="BH13" t="n" s="4">
@@ -5359,7 +5359,7 @@
       <c r="BM13" t="n" s="4">
         <v>24.0</v>
       </c>
-      <c r="BN13" t="n">
+      <c r="BN13" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO13" t="n" s="4">
@@ -5374,7 +5374,7 @@
       <c r="BR13" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS13" t="n">
+      <c r="BS13" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT13" t="n" s="4">
@@ -5389,7 +5389,7 @@
       <c r="BW13" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX13" t="n">
+      <c r="BX13" t="n" s="4">
         <v>8.0</v>
       </c>
       <c r="BY13" t="n" s="4">
@@ -5410,7 +5410,7 @@
       <c r="CD13" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE13" t="n">
+      <c r="CE13" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF13" t="n" s="4">
@@ -5442,7 +5442,7 @@
       <c r="C14" t="n" s="4">
         <v>36.0</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14" t="n" s="4">
         <v>36.0</v>
       </c>
       <c r="E14" t="n" s="4">
@@ -5469,7 +5469,7 @@
       <c r="L14" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M14" t="n">
+      <c r="M14" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N14" t="n" s="4">
@@ -5484,7 +5484,7 @@
       <c r="Q14" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R14" t="n">
+      <c r="R14" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S14" t="n" s="4">
@@ -5496,7 +5496,7 @@
       <c r="U14" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V14" t="n">
+      <c r="V14" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W14" t="n" s="4">
@@ -5511,7 +5511,7 @@
       <c r="Z14" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AA14" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB14" t="n" s="4">
@@ -5526,7 +5526,7 @@
       <c r="AE14" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF14" t="n">
+      <c r="AF14" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG14" t="n" s="4">
@@ -5535,7 +5535,7 @@
       <c r="AH14" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI14" t="n">
+      <c r="AI14" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ14" t="n" s="4">
@@ -5544,7 +5544,7 @@
       <c r="AK14" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL14" t="n">
+      <c r="AL14" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM14" t="n" s="4">
@@ -5562,7 +5562,7 @@
       <c r="AQ14" t="n" s="4">
         <v>51.0</v>
       </c>
-      <c r="AR14" t="n">
+      <c r="AR14" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS14" t="n" s="4">
@@ -5580,7 +5580,7 @@
       <c r="AW14" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX14" t="n">
+      <c r="AX14" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY14" t="n" s="4">
@@ -5607,7 +5607,7 @@
       <c r="BF14" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG14" t="n">
+      <c r="BG14" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH14" t="n" s="4">
@@ -5628,7 +5628,7 @@
       <c r="BM14" t="n" s="4">
         <v>39.0</v>
       </c>
-      <c r="BN14" t="n">
+      <c r="BN14" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO14" t="n" s="4">
@@ -5643,7 +5643,7 @@
       <c r="BR14" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS14" t="n">
+      <c r="BS14" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="BT14" t="n" s="4">
@@ -5658,7 +5658,7 @@
       <c r="BW14" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX14" t="n">
+      <c r="BX14" t="n" s="4">
         <v>13.0</v>
       </c>
       <c r="BY14" t="n" s="4">
@@ -5679,7 +5679,7 @@
       <c r="CD14" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE14" t="n">
+      <c r="CE14" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF14" t="n" s="4">
@@ -5711,7 +5711,7 @@
       <c r="C15" t="n" s="4">
         <v>36.0</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15" t="n" s="4">
         <v>36.0</v>
       </c>
       <c r="E15" t="n" s="4">
@@ -5738,7 +5738,7 @@
       <c r="L15" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M15" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N15" t="n" s="4">
@@ -5753,7 +5753,7 @@
       <c r="Q15" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R15" t="n">
+      <c r="R15" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S15" t="n" s="4">
@@ -5765,7 +5765,7 @@
       <c r="U15" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V15" t="n">
+      <c r="V15" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W15" t="n" s="4">
@@ -5780,7 +5780,7 @@
       <c r="Z15" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AA15" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB15" t="n" s="4">
@@ -5795,7 +5795,7 @@
       <c r="AE15" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF15" t="n">
+      <c r="AF15" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG15" t="n" s="4">
@@ -5804,7 +5804,7 @@
       <c r="AH15" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI15" t="n">
+      <c r="AI15" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ15" t="n" s="4">
@@ -5813,7 +5813,7 @@
       <c r="AK15" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL15" t="n">
+      <c r="AL15" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM15" t="n" s="4">
@@ -5831,7 +5831,7 @@
       <c r="AQ15" t="n" s="4">
         <v>58.0</v>
       </c>
-      <c r="AR15" t="n">
+      <c r="AR15" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS15" t="n" s="4">
@@ -5849,7 +5849,7 @@
       <c r="AW15" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX15" t="n">
+      <c r="AX15" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY15" t="n" s="4">
@@ -5876,7 +5876,7 @@
       <c r="BF15" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG15" t="n">
+      <c r="BG15" t="n" s="4">
         <v>33.0</v>
       </c>
       <c r="BH15" t="n" s="4">
@@ -5897,7 +5897,7 @@
       <c r="BM15" t="n" s="4">
         <v>27.0</v>
       </c>
-      <c r="BN15" t="n">
+      <c r="BN15" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO15" t="n" s="4">
@@ -5912,7 +5912,7 @@
       <c r="BR15" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS15" t="n">
+      <c r="BS15" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT15" t="n" s="4">
@@ -5927,7 +5927,7 @@
       <c r="BW15" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX15" t="n">
+      <c r="BX15" t="n" s="4">
         <v>8.0</v>
       </c>
       <c r="BY15" t="n" s="4">
@@ -5948,7 +5948,7 @@
       <c r="CD15" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE15" t="n">
+      <c r="CE15" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF15" t="n" s="4">
@@ -5980,7 +5980,7 @@
       <c r="C16" t="n" s="4">
         <v>36.0</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16" t="n" s="4">
         <v>36.0</v>
       </c>
       <c r="E16" t="n" s="4">
@@ -6007,7 +6007,7 @@
       <c r="L16" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M16" t="n">
+      <c r="M16" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N16" t="n" s="4">
@@ -6022,7 +6022,7 @@
       <c r="Q16" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R16" t="n">
+      <c r="R16" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S16" t="n" s="4">
@@ -6034,7 +6034,7 @@
       <c r="U16" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V16" t="n">
+      <c r="V16" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W16" t="n" s="4">
@@ -6049,7 +6049,7 @@
       <c r="Z16" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AA16" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB16" t="n" s="4">
@@ -6064,7 +6064,7 @@
       <c r="AE16" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF16" t="n">
+      <c r="AF16" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG16" t="n" s="4">
@@ -6073,7 +6073,7 @@
       <c r="AH16" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI16" t="n">
+      <c r="AI16" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ16" t="n" s="4">
@@ -6082,7 +6082,7 @@
       <c r="AK16" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL16" t="n">
+      <c r="AL16" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM16" t="n" s="4">
@@ -6100,7 +6100,7 @@
       <c r="AQ16" t="n" s="4">
         <v>58.0</v>
       </c>
-      <c r="AR16" t="n">
+      <c r="AR16" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS16" t="n" s="4">
@@ -6118,7 +6118,7 @@
       <c r="AW16" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX16" t="n">
+      <c r="AX16" t="n" s="4">
         <v>40.0</v>
       </c>
       <c r="AY16" t="n" s="4">
@@ -6145,7 +6145,7 @@
       <c r="BF16" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG16" t="n">
+      <c r="BG16" t="n" s="4">
         <v>33.0</v>
       </c>
       <c r="BH16" t="n" s="4">
@@ -6166,7 +6166,7 @@
       <c r="BM16" t="n" s="4">
         <v>27.0</v>
       </c>
-      <c r="BN16" t="n">
+      <c r="BN16" t="n" s="4">
         <v>56.0</v>
       </c>
       <c r="BO16" t="n" s="4">
@@ -6181,7 +6181,7 @@
       <c r="BR16" t="n" s="4">
         <v>4.8</v>
       </c>
-      <c r="BS16" t="n">
+      <c r="BS16" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT16" t="n" s="4">
@@ -6196,7 +6196,7 @@
       <c r="BW16" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX16" t="n">
+      <c r="BX16" t="n" s="4">
         <v>8.0</v>
       </c>
       <c r="BY16" t="n" s="4">
@@ -6217,7 +6217,7 @@
       <c r="CD16" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE16" t="n">
+      <c r="CE16" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF16" t="n" s="4">
@@ -6249,7 +6249,7 @@
       <c r="C17" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E17" t="n" s="4">
@@ -6276,7 +6276,7 @@
       <c r="L17" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M17" t="n">
+      <c r="M17" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N17" t="n" s="4">
@@ -6291,7 +6291,7 @@
       <c r="Q17" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R17" t="n">
+      <c r="R17" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S17" t="n" s="4">
@@ -6303,7 +6303,7 @@
       <c r="U17" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V17" t="n">
+      <c r="V17" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W17" t="n" s="4">
@@ -6318,7 +6318,7 @@
       <c r="Z17" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AA17" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB17" t="n" s="4">
@@ -6333,7 +6333,7 @@
       <c r="AE17" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF17" t="n">
+      <c r="AF17" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG17" t="n" s="4">
@@ -6342,7 +6342,7 @@
       <c r="AH17" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI17" t="n">
+      <c r="AI17" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ17" t="n" s="4">
@@ -6351,7 +6351,7 @@
       <c r="AK17" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL17" t="n">
+      <c r="AL17" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM17" t="n" s="4">
@@ -6369,7 +6369,7 @@
       <c r="AQ17" t="n" s="4">
         <v>49.0</v>
       </c>
-      <c r="AR17" t="n">
+      <c r="AR17" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AS17" t="n" s="4">
@@ -6387,7 +6387,7 @@
       <c r="AW17" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX17" t="n">
+      <c r="AX17" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY17" t="n" s="4">
@@ -6414,7 +6414,7 @@
       <c r="BF17" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG17" t="n">
+      <c r="BG17" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH17" t="n" s="4">
@@ -6435,7 +6435,7 @@
       <c r="BM17" t="n" s="4">
         <v>23.0</v>
       </c>
-      <c r="BN17" t="n">
+      <c r="BN17" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO17" t="n" s="4">
@@ -6450,7 +6450,7 @@
       <c r="BR17" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS17" t="n">
+      <c r="BS17" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT17" t="n" s="4">
@@ -6465,7 +6465,7 @@
       <c r="BW17" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX17" t="n">
+      <c r="BX17" t="n" s="4">
         <v>4.0</v>
       </c>
       <c r="BY17" t="n" s="4">
@@ -6486,7 +6486,7 @@
       <c r="CD17" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE17" t="n">
+      <c r="CE17" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF17" t="n" s="4">
@@ -6518,7 +6518,7 @@
       <c r="C18" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E18" t="n" s="4">
@@ -6545,7 +6545,7 @@
       <c r="L18" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M18" t="n">
+      <c r="M18" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N18" t="n" s="4">
@@ -6560,7 +6560,7 @@
       <c r="Q18" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R18" t="n">
+      <c r="R18" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S18" t="n" s="4">
@@ -6572,7 +6572,7 @@
       <c r="U18" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V18" t="n">
+      <c r="V18" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W18" t="n" s="4">
@@ -6587,7 +6587,7 @@
       <c r="Z18" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AA18" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB18" t="n" s="4">
@@ -6602,7 +6602,7 @@
       <c r="AE18" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF18" t="n">
+      <c r="AF18" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG18" t="n" s="4">
@@ -6611,7 +6611,7 @@
       <c r="AH18" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI18" t="n">
+      <c r="AI18" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ18" t="n" s="4">
@@ -6620,7 +6620,7 @@
       <c r="AK18" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL18" t="n">
+      <c r="AL18" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM18" t="n" s="4">
@@ -6638,7 +6638,7 @@
       <c r="AQ18" t="n" s="4">
         <v>49.0</v>
       </c>
-      <c r="AR18" t="n">
+      <c r="AR18" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AS18" t="n" s="4">
@@ -6656,7 +6656,7 @@
       <c r="AW18" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX18" t="n">
+      <c r="AX18" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY18" t="n" s="4">
@@ -6683,7 +6683,7 @@
       <c r="BF18" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG18" t="n">
+      <c r="BG18" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH18" t="n" s="4">
@@ -6704,7 +6704,7 @@
       <c r="BM18" t="n" s="4">
         <v>25.0</v>
       </c>
-      <c r="BN18" t="n">
+      <c r="BN18" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO18" t="n" s="4">
@@ -6719,7 +6719,7 @@
       <c r="BR18" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS18" t="n">
+      <c r="BS18" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT18" t="n" s="4">
@@ -6734,7 +6734,7 @@
       <c r="BW18" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX18" t="n">
+      <c r="BX18" t="n" s="4">
         <v>13.0</v>
       </c>
       <c r="BY18" t="n" s="4">
@@ -6755,7 +6755,7 @@
       <c r="CD18" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE18" t="n">
+      <c r="CE18" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF18" t="n" s="4">
@@ -6787,7 +6787,7 @@
       <c r="C19" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E19" t="n" s="4">
@@ -6814,7 +6814,7 @@
       <c r="L19" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M19" t="n">
+      <c r="M19" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N19" t="n" s="4">
@@ -6829,7 +6829,7 @@
       <c r="Q19" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R19" t="n">
+      <c r="R19" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S19" t="n" s="4">
@@ -6841,7 +6841,7 @@
       <c r="U19" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V19" t="n">
+      <c r="V19" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W19" t="n" s="4">
@@ -6856,7 +6856,7 @@
       <c r="Z19" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AA19" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB19" t="n" s="4">
@@ -6871,7 +6871,7 @@
       <c r="AE19" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF19" t="n">
+      <c r="AF19" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG19" t="n" s="4">
@@ -6880,7 +6880,7 @@
       <c r="AH19" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI19" t="n">
+      <c r="AI19" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ19" t="n" s="4">
@@ -6889,7 +6889,7 @@
       <c r="AK19" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL19" t="n">
+      <c r="AL19" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM19" t="n" s="4">
@@ -6907,7 +6907,7 @@
       <c r="AQ19" t="n" s="4">
         <v>49.0</v>
       </c>
-      <c r="AR19" t="n">
+      <c r="AR19" t="n" s="4">
         <v>86.0</v>
       </c>
       <c r="AS19" t="n" s="4">
@@ -6925,7 +6925,7 @@
       <c r="AW19" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX19" t="n">
+      <c r="AX19" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY19" t="n" s="4">
@@ -6952,7 +6952,7 @@
       <c r="BF19" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG19" t="n">
+      <c r="BG19" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH19" t="n" s="4">
@@ -6973,7 +6973,7 @@
       <c r="BM19" t="n" s="4">
         <v>23.0</v>
       </c>
-      <c r="BN19" t="n">
+      <c r="BN19" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO19" t="n" s="4">
@@ -6988,7 +6988,7 @@
       <c r="BR19" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS19" t="n">
+      <c r="BS19" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT19" t="n" s="4">
@@ -7003,7 +7003,7 @@
       <c r="BW19" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX19" t="n">
+      <c r="BX19" t="n" s="4">
         <v>4.0</v>
       </c>
       <c r="BY19" t="n" s="4">
@@ -7024,7 +7024,7 @@
       <c r="CD19" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE19" t="n">
+      <c r="CE19" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF19" t="n" s="4">
@@ -7056,7 +7056,7 @@
       <c r="C20" t="n" s="4">
         <v>28.0</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20" t="n" s="4">
         <v>14.0</v>
       </c>
       <c r="E20" t="n" s="4">
@@ -7083,7 +7083,7 @@
       <c r="L20" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="M20" t="n">
+      <c r="M20" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="N20" t="n" s="4">
@@ -7098,7 +7098,7 @@
       <c r="Q20" t="n" s="4">
         <v>3.0</v>
       </c>
-      <c r="R20" t="n">
+      <c r="R20" t="n" s="4">
         <v>0.0</v>
       </c>
       <c r="S20" t="n" s="4">
@@ -7110,7 +7110,7 @@
       <c r="U20" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="V20" t="n">
+      <c r="V20" t="n" s="4">
         <v>12.0</v>
       </c>
       <c r="W20" t="n" s="4">
@@ -7125,7 +7125,7 @@
       <c r="Z20" t="n" s="4">
         <v>70.0</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AA20" t="n" s="4">
         <v>72.0</v>
       </c>
       <c r="AB20" t="n" s="4">
@@ -7140,7 +7140,7 @@
       <c r="AE20" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AF20" t="n">
+      <c r="AF20" t="n" s="4">
         <v>100.0</v>
       </c>
       <c r="AG20" t="n" s="4">
@@ -7149,7 +7149,7 @@
       <c r="AH20" t="n" s="4">
         <v>8.0</v>
       </c>
-      <c r="AI20" t="n">
+      <c r="AI20" t="n" s="4">
         <v>18.0</v>
       </c>
       <c r="AJ20" t="n" s="4">
@@ -7158,7 +7158,7 @@
       <c r="AK20" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AL20" t="n">
+      <c r="AL20" t="n" s="4">
         <v>85.0</v>
       </c>
       <c r="AM20" t="n" s="4">
@@ -7176,7 +7176,7 @@
       <c r="AQ20" t="n" s="4">
         <v>51.0</v>
       </c>
-      <c r="AR20" t="n">
+      <c r="AR20" t="n" s="4">
         <v>90.0</v>
       </c>
       <c r="AS20" t="n" s="4">
@@ -7194,7 +7194,7 @@
       <c r="AW20" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="AX20" t="n">
+      <c r="AX20" t="n" s="4">
         <v>25.0</v>
       </c>
       <c r="AY20" t="n" s="4">
@@ -7221,7 +7221,7 @@
       <c r="BF20" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BG20" t="n">
+      <c r="BG20" t="n" s="4">
         <v>24.0</v>
       </c>
       <c r="BH20" t="n" s="4">
@@ -7242,7 +7242,7 @@
       <c r="BM20" t="n" s="4">
         <v>25.0</v>
       </c>
-      <c r="BN20" t="n">
+      <c r="BN20" t="n" s="4">
         <v>41.0</v>
       </c>
       <c r="BO20" t="n" s="4">
@@ -7257,7 +7257,7 @@
       <c r="BR20" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="BS20" t="n">
+      <c r="BS20" t="n" s="4">
         <v>32.0</v>
       </c>
       <c r="BT20" t="n" s="4">
@@ -7272,7 +7272,7 @@
       <c r="BW20" t="n" s="4">
         <v>5.0</v>
       </c>
-      <c r="BX20" t="n">
+      <c r="BX20" t="n" s="4">
         <v>13.0</v>
       </c>
       <c r="BY20" t="n" s="4">
@@ -7293,7 +7293,7 @@
       <c r="CD20" t="n" s="4">
         <v>0.0</v>
       </c>
-      <c r="CE20" t="n">
+      <c r="CE20" t="n" s="4">
         <v>16.0</v>
       </c>
       <c r="CF20" t="n" s="4">

</xml_diff>